<commit_message>
adding updated Test Case and Test Documentation
</commit_message>
<xml_diff>
--- a/TestDocumentation.xlsx
+++ b/TestDocumentation.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suminatamang/Desktop/foundation-project/Foundation-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB772A9-FE9D-E045-AEDE-DF35AA6D61F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DC91FE-50D9-634D-9543-A74DC4E43DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19980" yWindow="-28280" windowWidth="34400" windowHeight="28300" activeTab="2" xr2:uid="{141FEBC7-81F7-1649-89A1-A4A279A11C24}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{141FEBC7-81F7-1649-89A1-A4A279A11C24}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
     <sheet name="Strategy" sheetId="2" r:id="rId2"/>
     <sheet name="schedule" sheetId="3" r:id="rId3"/>
     <sheet name="SRS" sheetId="4" r:id="rId4"/>
+    <sheet name="Acceptance Testing" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="146">
   <si>
     <t>Users should be able to open a new User account with the Planetarium</t>
   </si>
@@ -103,6 +104,12 @@
     <t xml:space="preserve">the user should be directed to the user home page </t>
   </si>
   <si>
+    <t>Equivalence Partition testing for the uniqueness of usernames</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error Guess Testing to see if the passwords are in plain text in the interface for the application a regular user would have access to </t>
+  </si>
+  <si>
     <t>ID:1</t>
   </si>
   <si>
@@ -292,9 +299,6 @@
     <t>Boundary analysis to see If the user is logged out after certain period of inactivity</t>
   </si>
   <si>
-    <t xml:space="preserve">Boundary Analysis for the maximum number of planets that can be removed. </t>
-  </si>
-  <si>
     <t>Equivalence Partition testing to try to delete the non-existing planets</t>
   </si>
   <si>
@@ -379,15 +383,9 @@
     <t xml:space="preserve">user adds image of the moon </t>
   </si>
   <si>
-    <t>Equivalence Partition testing (users with access to their own resources, users trying to access other user's resources)</t>
-  </si>
-  <si>
     <t>Boundary analysis for logged in user vs not logged in user</t>
   </si>
   <si>
-    <t>Boundary analysis for testing the name length limit(0,31)</t>
-  </si>
-  <si>
     <t>Boundary Analysis for the names character length limit</t>
   </si>
   <si>
@@ -397,18 +395,12 @@
     <t xml:space="preserve">Exploratory testing to see if the user can only interact with the resources they have added. </t>
   </si>
   <si>
-    <t xml:space="preserve">Equivalence Partition testing for the uniqueness of the added planets </t>
-  </si>
-  <si>
     <t>equivalence partition to test if duplicate moon is allowed. (moon and planet / add the same moon to a diferent planet)</t>
   </si>
   <si>
     <t xml:space="preserve">equivalance partition () moon belongs to the planet/ moon not belonging to the planet </t>
   </si>
   <si>
-    <t xml:space="preserve">equivalence partitioning:  valid user access / invalid user access </t>
-  </si>
-  <si>
     <t>Boundary analysis (image provided vs not provided)</t>
   </si>
   <si>
@@ -419,13 +411,79 @@
   </si>
   <si>
     <t>October 28th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boundary analysis to check for username/ password length </t>
+  </si>
+  <si>
+    <t>Exploratory Testing to see if passwords are in plain text in any places we have access to in the provided software</t>
+  </si>
+  <si>
+    <t>Error Guess Testing to perform Acceptance Testing for the Use Case</t>
+  </si>
+  <si>
+    <t>Boundary Analysis: Boundary between (deleteing their own planets / other planet not on their profile)</t>
+  </si>
+  <si>
+    <t>exploratory and error guessing testing to see if you can access the home page directly from the link given.</t>
+  </si>
+  <si>
+    <t>Exploratorty to test the session (log in /log out to check the resource remains the same for the same user.</t>
+  </si>
+  <si>
+    <t>Exploratory: Test with multiple users logged in at the same time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equivalence Partition testing for the uniqueness of the added planets.  </t>
+  </si>
+  <si>
+    <t>Boundary analysis for 1. testing the name length limit(0,31) 2. test with image and no image</t>
+  </si>
+  <si>
+    <t>exploratory testing: to confirm that the ownership of the planet added is maintained even when multiple users</t>
+  </si>
+  <si>
+    <t>Equivalence Partition: owner and non-owners. Only the owners can delete the planet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploratory Testing to see if the deleted planet is still displayed or not </t>
+  </si>
+  <si>
+    <t>error guessing to see if the moon is deleted as well.</t>
+  </si>
+  <si>
+    <t>on home page, after create account, there's no redirect button to go back to login, just need to go back or refresh the page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create an account button is too small </t>
+  </si>
+  <si>
+    <t>When no unique username is provided, "user already exists" is a better alert message than failed</t>
+  </si>
+  <si>
+    <t>equivalence partitioning:  logged in user acces and trying to access directly from the link</t>
+  </si>
+  <si>
+    <t>without logging out, when the user opens the loginpage, it shows empty login scrreen. Instead it should automatically show the home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user should be shown (show password) while entering password </t>
+  </si>
+  <si>
+    <t>When adding already existing planet, "Planet already exists" message should be displayed instead of  just failed.</t>
+  </si>
+  <si>
+    <t>When adding only photo. "Enter name of the planet" message should have been displayed instead of just failed.</t>
+  </si>
+  <si>
+    <t>When adding planet, "planet added" alert should have been displayed.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -505,6 +563,11 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow (Body)"/>
     </font>
   </fonts>
   <fills count="13">
@@ -622,7 +685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -703,6 +766,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1048,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D070171E-5B05-384B-9BD5-A72C7E0BC4B0}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B6"/>
+    <sheetView topLeftCell="A2" zoomScale="93" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1065,25 +1133,25 @@
   <sheetData>
     <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.2">
@@ -1117,19 +1185,19 @@
         <v>18</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D3" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="27" t="s">
         <v>88</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1137,37 +1205,35 @@
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="80" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="40" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
       <c r="B5" s="28"/>
       <c r="C5" s="27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E5" s="27"/>
-      <c r="F5" s="27" t="s">
-        <v>97</v>
-      </c>
+      <c r="F5" s="38"/>
       <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:9" ht="56" customHeight="1" x14ac:dyDescent="0.25">
@@ -1175,14 +1241,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="27" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E6" s="28"/>
-      <c r="F6" s="27"/>
+      <c r="F6" s="27" t="s">
+        <v>98</v>
+      </c>
       <c r="G6" s="28"/>
     </row>
     <row r="7" spans="1:9" ht="20" x14ac:dyDescent="0.25">
@@ -1193,19 +1261,19 @@
         <v>19</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="40" x14ac:dyDescent="0.25">
@@ -1213,22 +1281,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="40" x14ac:dyDescent="0.25">
@@ -1240,16 +1308,16 @@
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1260,19 +1328,19 @@
       </c>
       <c r="B10" s="30"/>
       <c r="C10" s="29" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1296,19 +1364,19 @@
         <v>19</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F12" s="32" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G12" s="32" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="40" x14ac:dyDescent="0.25">
@@ -1316,22 +1384,22 @@
         <v>5</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="40" x14ac:dyDescent="0.25">
@@ -1341,16 +1409,16 @@
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
       <c r="D14" s="31" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="40" x14ac:dyDescent="0.25">
@@ -1358,20 +1426,20 @@
         <v>10</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C15" s="31"/>
       <c r="D15" s="31" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="20" x14ac:dyDescent="0.25">
@@ -1387,31 +1455,31 @@
     </row>
     <row r="20" spans="1:2" ht="22" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B20" s="23"/>
     </row>
     <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B21" s="24"/>
     </row>
     <row r="22" spans="1:2" ht="22" x14ac:dyDescent="0.3">
       <c r="A22" s="34" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B22" s="22"/>
     </row>
     <row r="23" spans="1:2" ht="22" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B23" s="25"/>
     </row>
     <row r="24" spans="1:2" ht="22" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B24" s="26"/>
     </row>
@@ -1424,128 +1492,179 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1271F50E-9E68-2B46-8F6F-C5C713F411CB}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="C1" zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.1640625" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.1640625" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="40.6640625" customWidth="1"/>
+    <col min="1" max="1" width="52.6640625" customWidth="1"/>
+    <col min="2" max="2" width="41.1640625" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" customWidth="1"/>
+    <col min="5" max="5" width="35.83203125" customWidth="1"/>
+    <col min="6" max="6" width="32.5" customWidth="1"/>
+    <col min="7" max="7" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="35" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="C1" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="E1" s="37" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="F1" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="B4" s="36" t="s">
+      <c r="C6" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="F5" s="36"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1557,7 +1676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32A0D41-9ED0-FC44-ACBC-A1559D59BB3C}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1571,83 +1690,83 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D3" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1670,27 +1789,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1702,4 +1821,62 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87260F3-1DD4-CD4A-BD62-2E34C2BCCE20}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="69.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding the most updated documents
</commit_message>
<xml_diff>
--- a/TestDocumentation.xlsx
+++ b/TestDocumentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suminatamang/Desktop/foundation-project/Foundation-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DC91FE-50D9-634D-9543-A74DC4E43DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20717316-7D6A-784D-A9E3-3209CF9C7DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{141FEBC7-81F7-1649-89A1-A4A279A11C24}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{141FEBC7-81F7-1649-89A1-A4A279A11C24}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="153">
   <si>
     <t>Users should be able to open a new User account with the Planetarium</t>
   </si>
@@ -65,9 +65,6 @@
     <t>then the user should be given an alert saying their account has been created successfully</t>
   </si>
   <si>
-    <t>and the user should be redirected to the login page</t>
-  </si>
-  <si>
     <t>when the user provides an invalid name and/or password and clicks the create button</t>
   </si>
   <si>
@@ -209,15 +206,6 @@
     <t xml:space="preserve">given the user is on the home  page </t>
   </si>
   <si>
-    <t>the home page refreshes with new added planet</t>
-  </si>
-  <si>
-    <t>the planet is removed and the home page refreshes</t>
-  </si>
-  <si>
-    <t>the moon associated with the planet is removed too</t>
-  </si>
-  <si>
     <t>when invalid planet identifier is provided</t>
   </si>
   <si>
@@ -227,9 +215,6 @@
     <t xml:space="preserve">given the user is on the home page </t>
   </si>
   <si>
-    <t>the page refreshes and the added moon is displayed on home page</t>
-  </si>
-  <si>
     <t>Invalid moon data is provided</t>
   </si>
   <si>
@@ -239,15 +224,6 @@
     <t xml:space="preserve">stays on the home page </t>
   </si>
   <si>
-    <t>valid moon identifier is provided for deletion</t>
-  </si>
-  <si>
-    <t>the user gets a message "moon (name) is deleted.</t>
-  </si>
-  <si>
-    <t>the page refreshes and the moon is removed from the home page</t>
-  </si>
-  <si>
     <t>Invalid moon identifier is provided for deletion</t>
   </si>
   <si>
@@ -272,24 +248,6 @@
     <t>negative acceptance</t>
   </si>
   <si>
-    <t>ID: 2</t>
-  </si>
-  <si>
-    <t>ID: 3</t>
-  </si>
-  <si>
-    <t>ID: 4</t>
-  </si>
-  <si>
-    <t>ID: 5</t>
-  </si>
-  <si>
-    <t>ID: 6</t>
-  </si>
-  <si>
-    <t>ID: 7</t>
-  </si>
-  <si>
     <t>Error guess testing to see if the username and password is automatically remembered</t>
   </si>
   <si>
@@ -323,15 +281,9 @@
     <t>Planets should be “owned” by the user that added it to the Planetarium</t>
   </si>
   <si>
-    <t xml:space="preserve">Planets and moons should have unique names	</t>
-  </si>
-  <si>
     <t xml:space="preserve">	Planets and Moons should allow adding an associated image, but it is not required for the data to be added to the database</t>
   </si>
   <si>
-    <t xml:space="preserve">	Planets should be “owned” by the user that added it to the Planetarium</t>
-  </si>
-  <si>
     <t>Moons should be “owned” by the Planet the User adding the moon associated it with</t>
   </si>
   <si>
@@ -347,21 +299,6 @@
     <t>user gets invalid username/password message and stays on login page</t>
   </si>
   <si>
-    <t>users sees the list of planets and moons added to the planetarium</t>
-  </si>
-  <si>
-    <t>user provides mismatching name and sort type</t>
-  </si>
-  <si>
-    <t>User provides the matching name and sort type</t>
-  </si>
-  <si>
-    <t>user provides planet and moon names with in the character limit</t>
-  </si>
-  <si>
-    <t>user provides unique name for planets and moon</t>
-  </si>
-  <si>
     <t>user provides planet and moon names with beyond or below character limit</t>
   </si>
   <si>
@@ -371,27 +308,15 @@
     <t>the home page should give an alert displaying these errors</t>
   </si>
   <si>
-    <t>user provides the matching name and the celestial body type</t>
-  </si>
-  <si>
     <t>user provides different name and the celestial body type</t>
   </si>
   <si>
-    <t xml:space="preserve">user provides valid names to the moon </t>
-  </si>
-  <si>
-    <t xml:space="preserve">user adds image of the moon </t>
-  </si>
-  <si>
     <t>Boundary analysis for logged in user vs not logged in user</t>
   </si>
   <si>
     <t>Boundary Analysis for the names character length limit</t>
   </si>
   <si>
-    <t xml:space="preserve">Boundary Analysis for the maximum number of moons that can be removed. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Exploratory testing to see if the user can only interact with the resources they have added. </t>
   </si>
   <si>
@@ -404,9 +329,6 @@
     <t>Boundary analysis (image provided vs not provided)</t>
   </si>
   <si>
-    <t>exploratory and error guessing to trying to remove the moons ownded by a different planet.</t>
-  </si>
-  <si>
     <t>equivalence Partition testing(valid image files, invalid image files)</t>
   </si>
   <si>
@@ -431,9 +353,6 @@
     <t>Exploratorty to test the session (log in /log out to check the resource remains the same for the same user.</t>
   </si>
   <si>
-    <t>Exploratory: Test with multiple users logged in at the same time</t>
-  </si>
-  <si>
     <t xml:space="preserve">Equivalence Partition testing for the uniqueness of the added planets.  </t>
   </si>
   <si>
@@ -455,15 +374,9 @@
     <t>on home page, after create account, there's no redirect button to go back to login, just need to go back or refresh the page</t>
   </si>
   <si>
-    <t xml:space="preserve">create an account button is too small </t>
-  </si>
-  <si>
     <t>When no unique username is provided, "user already exists" is a better alert message than failed</t>
   </si>
   <si>
-    <t>equivalence partitioning:  logged in user acces and trying to access directly from the link</t>
-  </si>
-  <si>
     <t>without logging out, when the user opens the loginpage, it shows empty login scrreen. Instead it should automatically show the home page</t>
   </si>
   <si>
@@ -477,13 +390,121 @@
   </si>
   <si>
     <t>When adding planet, "planet added" alert should have been displayed.</t>
+  </si>
+  <si>
+    <t>Moons should be "owned" by the the Planet the User adding the moon associated it with</t>
+  </si>
+  <si>
+    <t>Planets and moons should have unique names</t>
+  </si>
+  <si>
+    <t>the user should see all the planet/moon added by the user</t>
+  </si>
+  <si>
+    <t>then the page should refresh with the added planets</t>
+  </si>
+  <si>
+    <t>the user selects Planet from the drop down menu, enters name and clicks delete</t>
+  </si>
+  <si>
+    <t>then the page should refresh after the planet is removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user selects Moon from the drop down menu, enters name, Photo(optional) and clicks submit </t>
+  </si>
+  <si>
+    <t>then the page should refresh with the added moon</t>
+  </si>
+  <si>
+    <t>the user selects Moon from the drop down menu, enters name and clicks delete</t>
+  </si>
+  <si>
+    <t>then the page should refresh after the moon is removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user provides invalid username and password </t>
+  </si>
+  <si>
+    <t>and doesn't see the planets and moon added</t>
+  </si>
+  <si>
+    <t>the user selects Planet from the drop down menu, enters name(valid character limit, unique), Photo(optional) and clicks submit</t>
+  </si>
+  <si>
+    <t>equivalence partitioning:  logged in user acces and not logged in user trying to access directly from the link</t>
+  </si>
+  <si>
+    <t>Exploratory: see if the moon is owned by the planet and both the resources have the same owner</t>
+  </si>
+  <si>
+    <t>Boundary Analysis (deleteing the moon that they own)</t>
+  </si>
+  <si>
+    <t>exploratory and error guessing to trying to remove the moons ownded by a different owner, see if the deleted planet is still displayed or not</t>
+  </si>
+  <si>
+    <t>Notes for acceptance testing</t>
+  </si>
+  <si>
+    <t>Notes for Acceptance Testing</t>
+  </si>
+  <si>
+    <t>Due to these issues, even though the intended use of service is intuitive and easy to use, the service doesn't provide the user with sense of security, and doesn't inspire confidence with so many critical issues. The home page is good with the good background of universe, but the login page of the application is not pleasing to look at and doesn't keep up with the theme of the app and the home page.</t>
+  </si>
+  <si>
+    <t>Is the intended use of the service intuitive?</t>
+  </si>
+  <si>
+    <t>Is the service easy to use?</t>
+  </si>
+  <si>
+    <t>Does the service inspire confidence?</t>
+  </si>
+  <si>
+    <t>Is the service pleasing to look at?</t>
+  </si>
+  <si>
+    <t>The app works as intended and performs the functions as requirements; however, it can be improved in many areas to make the user's experience easy and smooth. The intended use of the service is intuitive in general. The user can naturally navigate and use the service without following detailed instruction. However, the service doesn't inspire confidence beacause of security isssue being compromised. The service could also see some improvements in the User Interface.</t>
+  </si>
+  <si>
+    <t>As a general user, on the home page, "Create an Account" button should have been larger.</t>
+  </si>
+  <si>
+    <t>While typing the password, "show password" option should have been added, and required to enter the password again for confirmation</t>
+  </si>
+  <si>
+    <t>When the account is created, the display message shouldn't have shown the password which is a huge security issue</t>
+  </si>
+  <si>
+    <t>There should have been a link to take you back to the login page, or it should have taken the user directly to the home page</t>
+  </si>
+  <si>
+    <t>The alert messages when error occurs are vague and should be specific to let the user know about the issue like:</t>
+  </si>
+  <si>
+    <t>When adding already existing planet, "Planet already exists" message should be displayed instead of just failed.</t>
+  </si>
+  <si>
+    <t>When removing Planet/Moon, clear alert message with the reason and instruction should be displayed for the user.</t>
+  </si>
+  <si>
+    <t>When adding only photo. "Enter name of the Planet/Moon" should be displayed instead of just failed.</t>
+  </si>
+  <si>
+    <t>When adding duplicate values, "Resources already exist" messages should be displayed.</t>
+  </si>
+  <si>
+    <t>The Planet/Moon could be managed and sorted with sort by options, and related resources should have been displayed together.</t>
+  </si>
+  <si>
+    <t>Acceptane Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -537,25 +558,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -569,8 +575,50 @@
       <color theme="0"/>
       <name val="Aptos Narrow (Body)"/>
     </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF1F2328"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -643,6 +691,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -685,7 +739,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -708,22 +762,9 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -735,43 +776,84 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1114,374 +1196,478 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D070171E-5B05-384B-9BD5-A72C7E0BC4B0}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="93" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.6640625" customWidth="1"/>
-    <col min="2" max="2" width="50.83203125" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" customWidth="1"/>
-    <col min="4" max="4" width="44.5" customWidth="1"/>
-    <col min="5" max="5" width="40.83203125" customWidth="1"/>
-    <col min="6" max="6" width="38.5" customWidth="1"/>
-    <col min="7" max="7" width="43" customWidth="1"/>
+    <col min="1" max="1" width="102.1640625" customWidth="1"/>
+    <col min="2" max="2" width="75.5" customWidth="1"/>
+    <col min="3" max="3" width="84.6640625" customWidth="1"/>
+    <col min="4" max="4" width="96.6640625" customWidth="1"/>
+    <col min="5" max="5" width="86.5" customWidth="1"/>
+    <col min="6" max="6" width="94.33203125" customWidth="1"/>
+    <col min="7" max="7" width="93.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="23" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="D2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="F2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="21" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="28" t="s">
+      <c r="C3" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="29"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:9" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="29"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+    </row>
+    <row r="9" spans="1:9" ht="43" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="36"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+    </row>
+    <row r="10" spans="1:9" ht="23" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="27" t="s">
+      <c r="C10" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="23" x14ac:dyDescent="0.2">
+      <c r="A11" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="23" x14ac:dyDescent="0.2">
+      <c r="A12" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="46" x14ac:dyDescent="0.2">
+      <c r="A13" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="23" x14ac:dyDescent="0.2">
+      <c r="A14" s="38"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A15" s="40"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="22" x14ac:dyDescent="0.3">
+      <c r="A16" s="40"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+    </row>
+    <row r="17" spans="1:7" ht="23" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="23" x14ac:dyDescent="0.2">
+      <c r="A18" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="G3" s="27" t="s">
+      <c r="F18" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="23" x14ac:dyDescent="0.2">
+      <c r="A19" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="46" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>89</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="40" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="27"/>
-    </row>
-    <row r="6" spans="1:9" ht="56" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" s="28"/>
-    </row>
-    <row r="7" spans="1:9" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="40" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="G8" s="30" t="s">
+      <c r="E20" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="23" x14ac:dyDescent="0.2">
+      <c r="A21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+    </row>
+    <row r="22" spans="1:7" ht="22" x14ac:dyDescent="0.3">
+      <c r="A22" s="42"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+    </row>
+    <row r="23" spans="1:7" ht="22" x14ac:dyDescent="0.3">
+      <c r="A23" s="42"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+    </row>
+    <row r="24" spans="1:7" ht="22" x14ac:dyDescent="0.3">
+      <c r="A24" s="42"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="28" spans="1:7" ht="34" x14ac:dyDescent="0.4">
+      <c r="A28" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="21"/>
+    </row>
+    <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.4">
+      <c r="A29" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="22"/>
+    </row>
+    <row r="30" spans="1:7" ht="34" x14ac:dyDescent="0.4">
+      <c r="A30" s="23" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="40" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" s="29" t="s">
+      <c r="B30" s="20"/>
+    </row>
+    <row r="31" spans="1:7" ht="34" x14ac:dyDescent="0.4">
+      <c r="A31" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" ht="40" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="29" t="s">
+      <c r="B31" s="24"/>
+    </row>
+    <row r="32" spans="1:7" ht="34" x14ac:dyDescent="0.4">
+      <c r="A32" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="20" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-    </row>
-    <row r="12" spans="1:9" ht="20" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="40" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="40" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="40" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="G15" s="31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="20" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="20" spans="1:2" ht="22" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="23"/>
-    </row>
-    <row r="21" spans="1:2" ht="22" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="24"/>
-    </row>
-    <row r="22" spans="1:2" ht="22" x14ac:dyDescent="0.3">
-      <c r="A22" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="22"/>
-    </row>
-    <row r="23" spans="1:2" ht="22" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="25"/>
-    </row>
-    <row r="24" spans="1:2" ht="22" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="26"/>
+      <c r="B32" s="25"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1494,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1271F50E-9E68-2B46-8F6F-C5C713F411CB}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="116" zoomScaleNormal="143" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1510,161 +1696,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="C1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>17</v>
+      <c r="B2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>132</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>116</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>119</v>
+        <v>20</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="G5" s="36" t="s">
-        <v>121</v>
+        <v>99</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>133</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="G6" s="36"/>
+        <v>21</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="16"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
+        <v>100</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1677,7 +1863,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1690,83 +1876,94 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="44" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="44" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="B5" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="14" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="B6" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="44" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="B7" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>48</v>
+      <c r="C7" s="46" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1788,28 +1985,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1825,58 +2022,246 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87260F3-1DD4-CD4A-BD62-2E34C2BCCE20}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A2:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="69.5" customWidth="1"/>
+    <col min="2" max="2" width="145" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35" customWidth="1"/>
+    <col min="5" max="5" width="51.6640625" customWidth="1"/>
+    <col min="6" max="6" width="35.5" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" customWidth="1"/>
+    <col min="8" max="8" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>145</v>
       </c>
     </row>
+    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding all the files
</commit_message>
<xml_diff>
--- a/TestDocumentation.xlsx
+++ b/TestDocumentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suminatamang/Desktop/foundation-project/Foundation-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20717316-7D6A-784D-A9E3-3209CF9C7DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7A3F37-C3E9-7044-8E4D-3102195652A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{141FEBC7-81F7-1649-89A1-A4A279A11C24}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{141FEBC7-81F7-1649-89A1-A4A279A11C24}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -1198,7 +1198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D070171E-5B05-384B-9BD5-A72C7E0BC4B0}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87260F3-1DD4-CD4A-BD62-2E34C2BCCE20}">
   <dimension ref="A2:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>